<commit_message>
modify dltfx for add ssq random choice func
</commit_message>
<xml_diff>
--- a/data/ssq.xlsx
+++ b/data/ssq.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27135" windowHeight="13140"/>
+    <workbookView windowWidth="26910" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5845,8 +5845,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0155865228595972"/>
-          <c:y val="0.282185177746535"/>
+          <c:x val="0.0163023766345328"/>
+          <c:y val="0.123348412188383"/>
           <c:w val="0.972482580891477"/>
           <c:h val="0.639566177947379"/>
         </c:manualLayout>
@@ -22650,8 +22650,8 @@
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -22660,7 +22660,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8816975" y="6578600"/>
-        <a:ext cx="13305790" cy="3161665"/>
+        <a:ext cx="13305790" cy="3695065"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -22993,8 +22993,8 @@
   <sheetPr/>
   <dimension ref="A1:U504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C463" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:M503"/>
+    <sheetView tabSelected="1" topLeftCell="E27" workbookViewId="0">
+      <selection activeCell="AC56" sqref="AC56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>